<commit_message>
fix: Update group type and classe to not null
</commit_message>
<xml_diff>
--- a/src/test/resources/level_room_teacher_teaching_unit_group.xlsx
+++ b/src/test/resources/level_room_teacher_teaching_unit_group.xlsx
@@ -5,7 +5,7 @@
   <fileSharing readOnlyRecommended="0" userName="rivon0507"/>
   <workbookPr/>
   <bookViews>
-    <workbookView activeTab="2" xWindow="240" yWindow="60" windowWidth="0" windowHeight="0" tabRatio="500"/>
+    <workbookView activeTab="4" xWindow="240" yWindow="60" windowWidth="0" windowHeight="0" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="level" sheetId="1" r:id="rId4"/>
@@ -17,17 +17,17 @@
   <calcPr/>
   <extLst>
     <ext uri="smNativeData">
-      <pm:revision xmlns:pm="smNativeData" day="1762207256" val="1228" rev="124" rev64="64" revOS="3" revMin="124" revMax="0"/>
-      <pm:docPrefs xmlns:pm="smNativeData" id="1762207256" fixedDigits="0" showNotice="1" showFrameBounds="1" autoChart="1" recalcOnPrint="1" recalcOnCopy="1" finalRounding="1" compatTextArt="1" tab="567" useDefinedPrintRange="1" printArea="currentSheet"/>
-      <pm:compatibility xmlns:pm="smNativeData" id="1762207256" overlapCells="1"/>
-      <pm:defCurrency xmlns:pm="smNativeData" id="1762207256"/>
+      <pm:revision xmlns:pm="smNativeData" day="1762365294" val="1228" rev="124" rev64="64" revOS="3" revMin="124" revMax="0"/>
+      <pm:docPrefs xmlns:pm="smNativeData" id="1762365294" fixedDigits="0" showNotice="1" showFrameBounds="1" autoChart="1" recalcOnPrint="1" recalcOnCopy="1" finalRounding="1" compatTextArt="1" tab="567" useDefinedPrintRange="1" printArea="currentSheet"/>
+      <pm:compatibility xmlns:pm="smNativeData" id="1762365294" overlapCells="1"/>
+      <pm:defCurrency xmlns:pm="smNativeData" id="1762365294"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="64">
   <si>
     <t>id</t>
   </si>
@@ -182,10 +182,22 @@
     <t>Langage C</t>
   </si>
   <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>classe</t>
+  </si>
+  <si>
     <t>20</t>
   </si>
   <si>
     <t>L1Gp1</t>
+  </si>
+  <si>
+    <t>CM</t>
+  </si>
+  <si>
+    <t>GB</t>
   </si>
   <si>
     <t>21</t>
@@ -231,7 +243,7 @@
       <sz val="10"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1762207256" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1762365294" ulstyle="none" kern="1">
             <pm:latin face="Basic Sans" sz="200" lang="default"/>
             <pm:cs face="Basic Roman" sz="200" lang="default"/>
             <pm:ea face="Basic Roman" sz="200" lang="default"/>
@@ -246,7 +258,7 @@
       <sz val="11"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1762207256" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1762365294" ulstyle="none" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Basic Roman" sz="220" lang="default"/>
             <pm:ea face="Basic Roman" sz="220" lang="default"/>
@@ -255,15 +267,26 @@
       </extLst>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFFFFFFF"/>
+        <extLst>
+          <ext uri="smNativeData">
+            <pm:shade xmlns:pm="smNativeData" id="1762365294" type="1" fgLvl="100" fgClr="00FFFFFF" bgLvl="100" bgClr="00000000"/>
+          </ext>
+        </extLst>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left style="none">
         <color rgb="FF000000"/>
@@ -279,7 +302,26 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1762207256"/>
+          <pm:border xmlns:pm="smNativeData" id="1762365294"/>
+        </ext>
+      </extLst>
+    </border>
+    <border>
+      <left style="none">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="none">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="none">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="none">
+        <color rgb="FF000000"/>
+      </bottom>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:border xmlns:pm="smNativeData" id="1762365294"/>
         </ext>
       </extLst>
     </border>
@@ -297,7 +339,7 @@
   <tableStyles count="0"/>
   <extLst>
     <ext uri="smNativeData">
-      <pm:charStyles xmlns:pm="smNativeData" id="1762207256" count="1">
+      <pm:charStyles xmlns:pm="smNativeData" id="1762365294" count="1">
         <pm:charStyle name="Normal" fontId="0" Id="1"/>
       </pm:charStyles>
     </ext>
@@ -617,7 +659,7 @@
   <printOptions>
     <extLst>
       <ext uri="smNativeData">
-        <pm:pageFlags xmlns:pm="smNativeData" id="1762207256" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+        <pm:pageFlags xmlns:pm="smNativeData" id="1762365294" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
       </ext>
     </extLst>
   </printOptions>
@@ -626,14 +668,14 @@
   <headerFooter>
     <extLst>
       <ext uri="smNativeData">
-        <pm:header xmlns:pm="smNativeData" id="1762207256" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
-        <pm:footer xmlns:pm="smNativeData" id="1762207256" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+        <pm:header xmlns:pm="smNativeData" id="1762365294" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1762365294" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
       </ext>
     </extLst>
   </headerFooter>
   <extLst>
     <ext uri="smNativeData">
-      <pm:sheetPrefs xmlns:pm="smNativeData" day="1762207256" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1762365294" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
         <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
         <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
       </pm:sheetPrefs>
@@ -754,7 +796,7 @@
   <printOptions>
     <extLst>
       <ext uri="smNativeData">
-        <pm:pageFlags xmlns:pm="smNativeData" id="1762207256" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+        <pm:pageFlags xmlns:pm="smNativeData" id="1762365294" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
       </ext>
     </extLst>
   </printOptions>
@@ -763,14 +805,14 @@
   <headerFooter>
     <extLst>
       <ext uri="smNativeData">
-        <pm:header xmlns:pm="smNativeData" id="1762207256" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
-        <pm:footer xmlns:pm="smNativeData" id="1762207256" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+        <pm:header xmlns:pm="smNativeData" id="1762365294" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1762365294" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
       </ext>
     </extLst>
   </headerFooter>
   <extLst>
     <ext uri="smNativeData">
-      <pm:sheetPrefs xmlns:pm="smNativeData" day="1762207256" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1762365294" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
         <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
         <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
       </pm:sheetPrefs>
@@ -783,7 +825,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="normal" workbookViewId="0">
+    <sheetView view="normal" workbookViewId="0">
       <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
@@ -900,7 +942,7 @@
   <printOptions>
     <extLst>
       <ext uri="smNativeData">
-        <pm:pageFlags xmlns:pm="smNativeData" id="1762207256" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+        <pm:pageFlags xmlns:pm="smNativeData" id="1762365294" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
       </ext>
     </extLst>
   </printOptions>
@@ -909,14 +951,14 @@
   <headerFooter>
     <extLst>
       <ext uri="smNativeData">
-        <pm:header xmlns:pm="smNativeData" id="1762207256" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
-        <pm:footer xmlns:pm="smNativeData" id="1762207256" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+        <pm:header xmlns:pm="smNativeData" id="1762365294" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1762365294" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
       </ext>
     </extLst>
   </headerFooter>
   <extLst>
     <ext uri="smNativeData">
-      <pm:sheetPrefs xmlns:pm="smNativeData" day="1762207256" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1762365294" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
         <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
         <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
       </pm:sheetPrefs>
@@ -1093,7 +1135,7 @@
   <printOptions>
     <extLst>
       <ext uri="smNativeData">
-        <pm:pageFlags xmlns:pm="smNativeData" id="1762207256" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+        <pm:pageFlags xmlns:pm="smNativeData" id="1762365294" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
       </ext>
     </extLst>
   </printOptions>
@@ -1102,14 +1144,14 @@
   <headerFooter>
     <extLst>
       <ext uri="smNativeData">
-        <pm:header xmlns:pm="smNativeData" id="1762207256" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
-        <pm:footer xmlns:pm="smNativeData" id="1762207256" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+        <pm:header xmlns:pm="smNativeData" id="1762365294" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1762365294" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
       </ext>
     </extLst>
   </headerFooter>
   <extLst>
     <ext uri="smNativeData">
-      <pm:sheetPrefs xmlns:pm="smNativeData" day="1762207256" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1762365294" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
         <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
         <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
       </pm:sheetPrefs>
@@ -1120,15 +1162,15 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView view="normal" workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" view="normal" workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.45"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1141,13 +1183,19 @@
       <c r="D1" s="1" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="2" spans="1:4">
+      <c r="E1" t="s">
+        <v>51</v>
+      </c>
+      <c r="F1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2" s="1" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>11</v>
@@ -1155,27 +1203,39 @@
       <c r="D2" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:4">
+      <c r="E2" t="s">
+        <v>55</v>
+      </c>
+      <c r="F2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3" s="1" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:4">
+      <c r="E3" t="s">
+        <v>55</v>
+      </c>
+      <c r="F3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
       <c r="A4" s="1" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>16</v>
@@ -1183,26 +1243,38 @@
       <c r="D4" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="5" spans="1:4">
+      <c r="E4" t="s">
+        <v>55</v>
+      </c>
+      <c r="F4" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
       <c r="A5" s="1" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>5</v>
+      </c>
+      <c r="E5" t="s">
+        <v>55</v>
+      </c>
+      <c r="F5" t="s">
+        <v>56</v>
       </c>
     </row>
   </sheetData>
   <printOptions>
     <extLst>
       <ext uri="smNativeData">
-        <pm:pageFlags xmlns:pm="smNativeData" id="1762207256" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+        <pm:pageFlags xmlns:pm="smNativeData" id="1762365294" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
       </ext>
     </extLst>
   </printOptions>
@@ -1211,14 +1283,14 @@
   <headerFooter>
     <extLst>
       <ext uri="smNativeData">
-        <pm:header xmlns:pm="smNativeData" id="1762207256" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
-        <pm:footer xmlns:pm="smNativeData" id="1762207256" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+        <pm:header xmlns:pm="smNativeData" id="1762365294" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1762365294" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
       </ext>
     </extLst>
   </headerFooter>
   <extLst>
     <ext uri="smNativeData">
-      <pm:sheetPrefs xmlns:pm="smNativeData" day="1762207256" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1762365294" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
         <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
         <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
       </pm:sheetPrefs>

</xml_diff>